<commit_message>
New 4 apis related to projects are added into framework excel worksheet
</commit_message>
<xml_diff>
--- a/booksonline/FrameworkForJiraApi.xlsx
+++ b/booksonline/FrameworkForJiraApi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\Now\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B767EBE3-BFBA-4B0D-A46F-DF8A6DC015DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F331C088-93BD-40BF-AB56-7358C129B19B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2C462DE-B581-48D9-99D4-AC6A6E2A3CBA}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="__BW_TABLE_PROPERTIES">#REF!</definedName>
-    <definedName name="frameworkJiraApi">framework!$E$3:$G$204</definedName>
+    <definedName name="frameworkJiraApi">framework!$E$3:$H$209</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="621">
   <si>
     <t>Jira Resource</t>
   </si>
@@ -3649,6 +3649,54 @@
   </si>
   <si>
     <t>201. Issues</t>
+  </si>
+  <si>
+    <t>2.1 Isssues Assigned to current User across all projects</t>
+  </si>
+  <si>
+    <t>Returns issues from all project since your JQL does not include any project specific conditions.</t>
+  </si>
+  <si>
+    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee=currentuser()</t>
+  </si>
+  <si>
+    <t>Extract Information from JSON</t>
+  </si>
+  <si>
+    <t>2.2 Get all open issues by project</t>
+  </si>
+  <si>
+    <t>Get all open issues by project</t>
+  </si>
+  <si>
+    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee = 'akshay.dongave@boardwalktech.com' and project=10010 AND status in ("In Progress", "To Do") AND resolution = Unresolved order by updated DESC</t>
+  </si>
+  <si>
+    <t>2.3 Get all issue by issuetype in specific project</t>
+  </si>
+  <si>
+    <t>Get all issue by issuetype in specific project</t>
+  </si>
+  <si>
+    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee = 'akshay.dongave@boardwalktech.com' and project=10010 AND issuetype = Task AND status in ("In Progress", "To Do") AND resolution = Unresolved order by updated DESC</t>
+  </si>
+  <si>
+    <t>2.4 Get all unresolved issue by specific project</t>
+  </si>
+  <si>
+    <t>Get all unresolved issue by specific project</t>
+  </si>
+  <si>
+    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee in (currentUser()) AND project = UCW AND issuetype in standardIssueTypes() AND status in ("In Progress", "To Do") AND resolution = Unresolved ORDER BY created DESC</t>
+  </si>
+  <si>
+    <t>2.5 Get all resolved issue by specific project</t>
+  </si>
+  <si>
+    <t>Get all resolved issue by specific project</t>
+  </si>
+  <si>
+    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee in (currentUser()) AND project = UCW AND issuetype in standardIssueTypes() AND status in ("In Progress", "To Do") AND resolution = Done ORDER BY created DESC</t>
   </si>
 </sst>
 </file>
@@ -4043,10 +4091,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8241749-1F6A-48E6-B41D-93FEA9771075}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="E3:G204"/>
+  <dimension ref="E3:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4054,11 +4102,12 @@
     <col min="1" max="4" width="8.88671875" style="3"/>
     <col min="5" max="5" width="45.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="44.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="71.33203125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="44.77734375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="71.33203125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4068,8 +4117,11 @@
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E4" s="2" t="s">
         <v>404</v>
       </c>
@@ -4079,8 +4131,9 @@
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E5" s="2" t="s">
         <v>405</v>
       </c>
@@ -4090,2195 +4143,2455 @@
       <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E6" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E10" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="2" t="s">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="2" t="s">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="2" t="s">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E14" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="2" t="s">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="2" t="s">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E16" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="2" t="s">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E17" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="2" t="s">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E18" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="2" t="s">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E19" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="2" t="s">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E20" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E16" s="2" t="s">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E21" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E17" s="2" t="s">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E22" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E18" s="2" t="s">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E23" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="2" t="s">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E24" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="2" t="s">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E25" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="2" t="s">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="2" t="s">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E27" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="2" t="s">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E28" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E24" s="2" t="s">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E29" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E25" s="2" t="s">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E30" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E26" s="2" t="s">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E31" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E27" s="2" t="s">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E32" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E28" s="2" t="s">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E33" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E29" s="2" t="s">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E34" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E30" s="2" t="s">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E35" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E31" s="2" t="s">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E36" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E32" s="2" t="s">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E37" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E33" s="2" t="s">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E38" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E34" s="2" t="s">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E39" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E35" s="2" t="s">
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E40" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E36" s="2" t="s">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E41" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E37" s="2" t="s">
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E42" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E38" s="2" t="s">
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E43" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E39" s="2" t="s">
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E44" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E40" s="2" t="s">
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E45" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E41" s="2" t="s">
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E46" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E42" s="2" t="s">
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E47" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E43" s="2" t="s">
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E48" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E44" s="2" t="s">
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E49" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E45" s="2" t="s">
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E50" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E46" s="2" t="s">
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E51" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E47" s="2" t="s">
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E52" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E48" s="2" t="s">
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E53" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E49" s="2" t="s">
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E54" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E50" s="2" t="s">
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E55" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E51" s="2" t="s">
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E56" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E52" s="2" t="s">
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E57" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E53" s="2" t="s">
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E58" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E54" s="2" t="s">
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E59" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E55" s="2" t="s">
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E60" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E56" s="2" t="s">
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E61" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E57" s="2" t="s">
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E62" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E58" s="2" t="s">
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E63" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E59" s="2" t="s">
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E64" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G64" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E60" s="2" t="s">
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E65" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E61" s="2" t="s">
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E66" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E62" s="2" t="s">
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E67" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E63" s="2" t="s">
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E68" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E64" s="2" t="s">
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E69" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="65" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E65" s="2" t="s">
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E70" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="66" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E66" s="2" t="s">
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E71" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="67" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E67" s="2" t="s">
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E72" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="68" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E68" s="2" t="s">
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E73" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="69" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E69" s="2" t="s">
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E74" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="70" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E70" s="2" t="s">
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E75" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="71" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E71" s="2" t="s">
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E76" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="72" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E72" s="2" t="s">
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E77" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="73" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E73" s="2" t="s">
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E78" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="74" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E74" s="2" t="s">
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E79" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="75" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E75" s="2" t="s">
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E80" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="76" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E76" s="2" t="s">
+      <c r="H80" s="2"/>
+    </row>
+    <row r="81" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E81" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="77" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E77" s="2" t="s">
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E82" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="78" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E78" s="2" t="s">
+      <c r="H82" s="2"/>
+    </row>
+    <row r="83" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E83" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="79" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E79" s="2" t="s">
+      <c r="H83" s="2"/>
+    </row>
+    <row r="84" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E84" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G84" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="80" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E80" s="2" t="s">
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E85" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="G85" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="81" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E81" s="2" t="s">
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E86" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G86" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="82" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E82" s="2" t="s">
+      <c r="H86" s="2"/>
+    </row>
+    <row r="87" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E87" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="83" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E83" s="2" t="s">
+      <c r="H87" s="2"/>
+    </row>
+    <row r="88" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E88" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F88" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="84" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E84" s="2" t="s">
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E89" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F89" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="85" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E85" s="2" t="s">
+      <c r="H89" s="2"/>
+    </row>
+    <row r="90" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E90" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="86" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E86" s="2" t="s">
+      <c r="H90" s="2"/>
+    </row>
+    <row r="91" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E91" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F91" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="87" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E87" s="2" t="s">
+      <c r="H91" s="2"/>
+    </row>
+    <row r="92" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E92" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F92" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="88" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E88" s="2" t="s">
+      <c r="H92" s="2"/>
+    </row>
+    <row r="93" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E93" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G93" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="89" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E89" s="2" t="s">
+      <c r="H93" s="2"/>
+    </row>
+    <row r="94" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E94" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F94" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G94" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="90" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E90" s="2" t="s">
+      <c r="H94" s="2"/>
+    </row>
+    <row r="95" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E95" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="F95" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="G95" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="91" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E91" s="2" t="s">
+      <c r="H95" s="2"/>
+    </row>
+    <row r="96" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E96" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="F96" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="92" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E92" s="2" t="s">
+      <c r="H96" s="2"/>
+    </row>
+    <row r="97" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E97" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="F97" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="G97" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="93" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E93" s="2" t="s">
+      <c r="H97" s="2"/>
+    </row>
+    <row r="98" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E98" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G93" s="2" t="s">
+      <c r="G98" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="94" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E94" s="2" t="s">
+      <c r="H98" s="2"/>
+    </row>
+    <row r="99" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E99" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="F94" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="95" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E95" s="2" t="s">
+      <c r="H99" s="2"/>
+    </row>
+    <row r="100" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E100" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="96" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E96" s="2" t="s">
+      <c r="H100" s="2"/>
+    </row>
+    <row r="101" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E101" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="G101" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="97" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E97" s="2" t="s">
+      <c r="H101" s="2"/>
+    </row>
+    <row r="102" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E102" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G97" s="2" t="s">
+      <c r="G102" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="98" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E98" s="2" t="s">
+      <c r="H102" s="2"/>
+    </row>
+    <row r="103" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E103" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="99" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E99" s="2" t="s">
+      <c r="H103" s="2"/>
+    </row>
+    <row r="104" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E104" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="100" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E100" s="2" t="s">
+      <c r="H104" s="2"/>
+    </row>
+    <row r="105" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E105" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F105" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="G105" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="101" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E101" s="2" t="s">
+      <c r="H105" s="2"/>
+    </row>
+    <row r="106" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E106" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F106" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="G106" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="102" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E102" s="2" t="s">
+      <c r="H106" s="2"/>
+    </row>
+    <row r="107" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E107" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F107" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G107" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="103" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E103" s="2" t="s">
+      <c r="H107" s="2"/>
+    </row>
+    <row r="108" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E108" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F108" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="G103" s="2" t="s">
+      <c r="G108" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="104" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E104" s="2" t="s">
+      <c r="H108" s="2"/>
+    </row>
+    <row r="109" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E109" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="G109" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="105" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E105" s="2" t="s">
+      <c r="H109" s="2"/>
+    </row>
+    <row r="110" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E110" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="F105" s="2" t="s">
+      <c r="F110" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G105" s="2" t="s">
+      <c r="G110" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="106" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E106" s="2" t="s">
+      <c r="H110" s="2"/>
+    </row>
+    <row r="111" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E111" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F106" s="2" t="s">
+      <c r="F111" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G106" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="107" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E107" s="2" t="s">
+      <c r="H111" s="2"/>
+    </row>
+    <row r="112" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E112" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="F112" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G107" s="2" t="s">
+      <c r="G112" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="108" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E108" s="2" t="s">
+      <c r="H112" s="2"/>
+    </row>
+    <row r="113" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E113" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F113" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="G113" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="109" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E109" s="2" t="s">
+      <c r="H113" s="2"/>
+    </row>
+    <row r="114" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E114" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="F114" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="G114" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="110" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E110" s="2" t="s">
+      <c r="H114" s="2"/>
+    </row>
+    <row r="115" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E115" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="F115" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G110" s="2" t="s">
+      <c r="G115" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="111" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E111" s="2" t="s">
+      <c r="H115" s="2"/>
+    </row>
+    <row r="116" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E116" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="F116" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="G111" s="2" t="s">
+      <c r="G116" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="112" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E112" s="2" t="s">
+      <c r="H116" s="2"/>
+    </row>
+    <row r="117" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E117" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="F117" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G112" s="2" t="s">
+      <c r="G117" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="113" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E113" s="2" t="s">
+      <c r="H117" s="2"/>
+    </row>
+    <row r="118" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E118" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="F118" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="G113" s="2" t="s">
+      <c r="G118" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="114" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E114" s="2" t="s">
+      <c r="H118" s="2"/>
+    </row>
+    <row r="119" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E119" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F119" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G114" s="2" t="s">
+      <c r="G119" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="115" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E115" s="2" t="s">
+      <c r="H119" s="2"/>
+    </row>
+    <row r="120" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E120" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="F120" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G115" s="2" t="s">
+      <c r="G120" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="116" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E116" s="2" t="s">
+      <c r="H120" s="2"/>
+    </row>
+    <row r="121" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E121" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="F121" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="G121" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="117" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E117" s="2" t="s">
+      <c r="H121" s="2"/>
+    </row>
+    <row r="122" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E122" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="F122" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="G122" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="118" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E118" s="2" t="s">
+      <c r="H122" s="2"/>
+    </row>
+    <row r="123" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E123" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="F123" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="G123" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="119" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E119" s="2" t="s">
+      <c r="H123" s="2"/>
+    </row>
+    <row r="124" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E124" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="F124" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="G119" s="2" t="s">
+      <c r="G124" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="120" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E120" s="2" t="s">
+      <c r="H124" s="2"/>
+    </row>
+    <row r="125" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E125" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F125" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="G120" s="2" t="s">
+      <c r="G125" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="121" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E121" s="2" t="s">
+      <c r="H125" s="2"/>
+    </row>
+    <row r="126" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E126" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="F121" s="2" t="s">
+      <c r="F126" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="G121" s="2" t="s">
+      <c r="G126" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="122" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E122" s="2" t="s">
+      <c r="H126" s="2"/>
+    </row>
+    <row r="127" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E127" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="F122" s="2" t="s">
+      <c r="F127" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="G122" s="2" t="s">
+      <c r="G127" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="123" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E123" s="2" t="s">
+      <c r="H127" s="2"/>
+    </row>
+    <row r="128" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E128" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="F123" s="2" t="s">
+      <c r="F128" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G123" s="2" t="s">
+      <c r="G128" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="124" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E124" s="2" t="s">
+      <c r="H128" s="2"/>
+    </row>
+    <row r="129" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E129" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="F129" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="G129" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="125" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E125" s="2" t="s">
+      <c r="H129" s="2"/>
+    </row>
+    <row r="130" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E130" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="F125" s="2" t="s">
+      <c r="F130" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G125" s="2" t="s">
+      <c r="G130" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="126" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E126" s="2" t="s">
+      <c r="H130" s="2"/>
+    </row>
+    <row r="131" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E131" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="F126" s="2" t="s">
+      <c r="F131" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="G131" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="127" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E127" s="2" t="s">
+      <c r="H131" s="2"/>
+    </row>
+    <row r="132" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E132" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="F132" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="G127" s="2" t="s">
+      <c r="G132" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="128" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E128" s="2" t="s">
+      <c r="H132" s="2"/>
+    </row>
+    <row r="133" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E133" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="F133" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="G128" s="2" t="s">
+      <c r="G133" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="129" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E129" s="2" t="s">
+      <c r="H133" s="2"/>
+    </row>
+    <row r="134" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E134" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="F134" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G129" s="2" t="s">
+      <c r="G134" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="130" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E130" s="2" t="s">
+      <c r="H134" s="2"/>
+    </row>
+    <row r="135" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E135" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="F130" s="2" t="s">
+      <c r="F135" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G130" s="2" t="s">
+      <c r="G135" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="131" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E131" s="2" t="s">
+      <c r="H135" s="2"/>
+    </row>
+    <row r="136" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E136" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="F131" s="2" t="s">
+      <c r="F136" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G131" s="2" t="s">
+      <c r="G136" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="132" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E132" s="2" t="s">
+      <c r="H136" s="2"/>
+    </row>
+    <row r="137" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E137" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="F132" s="2" t="s">
+      <c r="F137" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="G132" s="2" t="s">
+      <c r="G137" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="133" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E133" s="2" t="s">
+      <c r="H137" s="2"/>
+    </row>
+    <row r="138" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E138" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="F133" s="2" t="s">
+      <c r="F138" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="G133" s="2" t="s">
+      <c r="G138" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="134" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E134" s="2" t="s">
+      <c r="H138" s="2"/>
+    </row>
+    <row r="139" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E139" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="F134" s="2" t="s">
+      <c r="F139" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G134" s="2" t="s">
+      <c r="G139" s="2" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="135" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E135" s="2" t="s">
+      <c r="H139" s="2"/>
+    </row>
+    <row r="140" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E140" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="F135" s="2" t="s">
+      <c r="F140" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="G135" s="2" t="s">
+      <c r="G140" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="136" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E136" s="2" t="s">
+      <c r="H140" s="2"/>
+    </row>
+    <row r="141" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E141" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="F136" s="2" t="s">
+      <c r="F141" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="G136" s="2" t="s">
+      <c r="G141" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="137" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E137" s="2" t="s">
+      <c r="H141" s="2"/>
+    </row>
+    <row r="142" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E142" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="F137" s="2" t="s">
+      <c r="F142" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="G137" s="2" t="s">
+      <c r="G142" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="138" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E138" s="2" t="s">
+      <c r="H142" s="2"/>
+    </row>
+    <row r="143" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E143" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="F138" s="2" t="s">
+      <c r="F143" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="G138" s="2" t="s">
+      <c r="G143" s="2" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="139" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E139" s="2" t="s">
+      <c r="H143" s="2"/>
+    </row>
+    <row r="144" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E144" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="F139" s="2" t="s">
+      <c r="F144" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="G139" s="2" t="s">
+      <c r="G144" s="2" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="140" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E140" s="2" t="s">
+      <c r="H144" s="2"/>
+    </row>
+    <row r="145" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E145" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="F140" s="2" t="s">
+      <c r="F145" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G140" s="2" t="s">
+      <c r="G145" s="2" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="141" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E141" s="2" t="s">
+      <c r="H145" s="2"/>
+    </row>
+    <row r="146" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E146" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="F141" s="2" t="s">
+      <c r="F146" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G141" s="2" t="s">
+      <c r="G146" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="142" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E142" s="2" t="s">
+      <c r="H146" s="2"/>
+    </row>
+    <row r="147" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E147" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="F142" s="2" t="s">
+      <c r="F147" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G142" s="2" t="s">
+      <c r="G147" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="143" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E143" s="2" t="s">
+      <c r="H147" s="2"/>
+    </row>
+    <row r="148" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E148" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="F143" s="2" t="s">
+      <c r="F148" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G143" s="2" t="s">
+      <c r="G148" s="2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="144" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E144" s="2" t="s">
+      <c r="H148" s="2"/>
+    </row>
+    <row r="149" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E149" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="F144" s="2" t="s">
+      <c r="F149" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G144" s="2" t="s">
+      <c r="G149" s="2" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="145" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E145" s="2" t="s">
+      <c r="H149" s="2"/>
+    </row>
+    <row r="150" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E150" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="F145" s="2" t="s">
+      <c r="F150" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="G145" s="2" t="s">
+      <c r="G150" s="2" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="146" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E146" s="2" t="s">
+      <c r="H150" s="2"/>
+    </row>
+    <row r="151" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E151" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="F146" s="2" t="s">
+      <c r="F151" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G146" s="2" t="s">
+      <c r="G151" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="147" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E147" s="2" t="s">
+      <c r="H151" s="2"/>
+    </row>
+    <row r="152" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E152" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="F147" s="2" t="s">
+      <c r="F152" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="G147" s="2" t="s">
+      <c r="G152" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="148" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E148" s="2" t="s">
+      <c r="H152" s="2"/>
+    </row>
+    <row r="153" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E153" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="F148" s="2" t="s">
+      <c r="F153" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="G148" s="2" t="s">
+      <c r="G153" s="2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="149" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E149" s="2" t="s">
+      <c r="H153" s="2"/>
+    </row>
+    <row r="154" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E154" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="F149" s="2" t="s">
+      <c r="F154" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="G149" s="2" t="s">
+      <c r="G154" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="150" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E150" s="2" t="s">
+      <c r="H154" s="2"/>
+    </row>
+    <row r="155" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E155" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="F150" s="2" t="s">
+      <c r="F155" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="G150" s="2" t="s">
+      <c r="G155" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="151" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E151" s="2" t="s">
+      <c r="H155" s="2"/>
+    </row>
+    <row r="156" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E156" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="F151" s="2" t="s">
+      <c r="F156" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="G151" s="2" t="s">
+      <c r="G156" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="152" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E152" s="2" t="s">
+      <c r="H156" s="2"/>
+    </row>
+    <row r="157" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E157" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="F152" s="2" t="s">
+      <c r="F157" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="G152" s="2" t="s">
+      <c r="G157" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="153" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E153" s="2" t="s">
+      <c r="H157" s="2"/>
+    </row>
+    <row r="158" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E158" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="F153" s="2" t="s">
+      <c r="F158" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="G153" s="2" t="s">
+      <c r="G158" s="2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="154" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E154" s="2" t="s">
+      <c r="H158" s="2"/>
+    </row>
+    <row r="159" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E159" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="F154" s="2" t="s">
+      <c r="F159" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="G154" s="2" t="s">
+      <c r="G159" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="155" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E155" s="2" t="s">
+      <c r="H159" s="2"/>
+    </row>
+    <row r="160" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E160" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="F155" s="2" t="s">
+      <c r="F160" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="G155" s="2" t="s">
+      <c r="G160" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="156" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E156" s="2" t="s">
+      <c r="H160" s="2"/>
+    </row>
+    <row r="161" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E161" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="F156" s="2" t="s">
+      <c r="F161" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G156" s="2" t="s">
+      <c r="G161" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="157" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E157" s="2" t="s">
+      <c r="H161" s="2"/>
+    </row>
+    <row r="162" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E162" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="F157" s="2" t="s">
+      <c r="F162" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="G157" s="2" t="s">
+      <c r="G162" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="158" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E158" s="2" t="s">
+      <c r="H162" s="2"/>
+    </row>
+    <row r="163" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E163" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="F158" s="2" t="s">
+      <c r="F163" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="G158" s="2" t="s">
+      <c r="G163" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="159" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E159" s="2" t="s">
+      <c r="H163" s="2"/>
+    </row>
+    <row r="164" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E164" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="F159" s="2" t="s">
+      <c r="F164" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="G159" s="2" t="s">
+      <c r="G164" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="160" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E160" s="2" t="s">
+      <c r="H164" s="2"/>
+    </row>
+    <row r="165" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E165" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="F160" s="2" t="s">
+      <c r="F165" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="G160" s="2" t="s">
+      <c r="G165" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="161" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E161" s="2" t="s">
+      <c r="H165" s="2"/>
+    </row>
+    <row r="166" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E166" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="F161" s="2" t="s">
+      <c r="F166" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="G161" s="2" t="s">
+      <c r="G166" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="162" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E162" s="2" t="s">
+      <c r="H166" s="2"/>
+    </row>
+    <row r="167" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E167" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="F162" s="2" t="s">
+      <c r="F167" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="G162" s="2" t="s">
+      <c r="G167" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="163" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E163" s="2" t="s">
+      <c r="H167" s="2"/>
+    </row>
+    <row r="168" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E168" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="F163" s="2" t="s">
+      <c r="F168" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="G163" s="2" t="s">
+      <c r="G168" s="2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="164" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E164" s="2" t="s">
+      <c r="H168" s="2"/>
+    </row>
+    <row r="169" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E169" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="F164" s="2" t="s">
+      <c r="F169" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="G164" s="2" t="s">
+      <c r="G169" s="2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="165" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E165" s="2" t="s">
+      <c r="H169" s="2"/>
+    </row>
+    <row r="170" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E170" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="F165" s="2" t="s">
+      <c r="F170" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="G165" s="2" t="s">
+      <c r="G170" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="166" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E166" s="2" t="s">
+      <c r="H170" s="2"/>
+    </row>
+    <row r="171" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E171" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="F166" s="2" t="s">
+      <c r="F171" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="G166" s="2" t="s">
+      <c r="G171" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="167" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E167" s="2" t="s">
+      <c r="H171" s="2"/>
+    </row>
+    <row r="172" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E172" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="F167" s="2" t="s">
+      <c r="F172" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G167" s="2" t="s">
+      <c r="G172" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="168" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E168" s="2" t="s">
+      <c r="H172" s="2"/>
+    </row>
+    <row r="173" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E173" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="F168" s="2" t="s">
+      <c r="F173" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="G168" s="2" t="s">
+      <c r="G173" s="2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="169" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E169" s="2" t="s">
+      <c r="H173" s="2"/>
+    </row>
+    <row r="174" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E174" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="F169" s="2" t="s">
+      <c r="F174" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="G169" s="2" t="s">
+      <c r="G174" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="170" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E170" s="2" t="s">
+      <c r="H174" s="2"/>
+    </row>
+    <row r="175" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E175" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="F170" s="2" t="s">
+      <c r="F175" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="G170" s="2" t="s">
+      <c r="G175" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="171" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E171" s="2" t="s">
+      <c r="H175" s="2"/>
+    </row>
+    <row r="176" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E176" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="F171" s="2" t="s">
+      <c r="F176" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="G171" s="2" t="s">
+      <c r="G176" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="172" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E172" s="2" t="s">
+      <c r="H176" s="2"/>
+    </row>
+    <row r="177" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E177" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="F172" s="2" t="s">
+      <c r="F177" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="G172" s="2" t="s">
+      <c r="G177" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="173" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E173" s="2" t="s">
+      <c r="H177" s="2"/>
+    </row>
+    <row r="178" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E178" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="F173" s="2" t="s">
+      <c r="F178" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="G173" s="2" t="s">
+      <c r="G178" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="174" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E174" s="2" t="s">
+      <c r="H178" s="2"/>
+    </row>
+    <row r="179" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E179" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="F174" s="2" t="s">
+      <c r="F179" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="G174" s="2" t="s">
+      <c r="G179" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="175" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E175" s="2" t="s">
+      <c r="H179" s="2"/>
+    </row>
+    <row r="180" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E180" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="F175" s="2" t="s">
+      <c r="F180" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="G175" s="2" t="s">
+      <c r="G180" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="176" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E176" s="2" t="s">
+      <c r="H180" s="2"/>
+    </row>
+    <row r="181" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E181" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="F176" s="2" t="s">
+      <c r="F181" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="G176" s="2" t="s">
+      <c r="G181" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="177" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E177" s="2" t="s">
+      <c r="H181" s="2"/>
+    </row>
+    <row r="182" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E182" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="F177" s="2" t="s">
+      <c r="F182" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="G177" s="2" t="s">
+      <c r="G182" s="2" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="178" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E178" s="2" t="s">
+      <c r="H182" s="2"/>
+    </row>
+    <row r="183" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E183" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="F178" s="2" t="s">
+      <c r="F183" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G178" s="2" t="s">
+      <c r="G183" s="2" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="179" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E179" s="2" t="s">
+      <c r="H183" s="2"/>
+    </row>
+    <row r="184" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E184" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="F179" s="2" t="s">
+      <c r="F184" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="G179" s="2" t="s">
+      <c r="G184" s="2" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="180" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E180" s="2" t="s">
+      <c r="H184" s="2"/>
+    </row>
+    <row r="185" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E185" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="F180" s="2" t="s">
+      <c r="F185" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="G180" s="2" t="s">
+      <c r="G185" s="2" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="181" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E181" s="2" t="s">
+      <c r="H185" s="2"/>
+    </row>
+    <row r="186" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E186" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="F181" s="2" t="s">
+      <c r="F186" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G181" s="2" t="s">
+      <c r="G186" s="2" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="182" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E182" s="2" t="s">
+      <c r="H186" s="2"/>
+    </row>
+    <row r="187" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E187" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="F182" s="2" t="s">
+      <c r="F187" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="G182" s="2" t="s">
+      <c r="G187" s="2" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="183" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E183" s="2" t="s">
+      <c r="H187" s="2"/>
+    </row>
+    <row r="188" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E188" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="F183" s="2" t="s">
+      <c r="F188" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="G183" s="2" t="s">
+      <c r="G188" s="2" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="184" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E184" s="2" t="s">
+      <c r="H188" s="2"/>
+    </row>
+    <row r="189" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E189" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="F184" s="2" t="s">
+      <c r="F189" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="G184" s="2" t="s">
+      <c r="G189" s="2" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="185" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E185" s="2" t="s">
+      <c r="H189" s="2"/>
+    </row>
+    <row r="190" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E190" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="F185" s="2" t="s">
+      <c r="F190" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="G185" s="2" t="s">
+      <c r="G190" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="186" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E186" s="2" t="s">
+      <c r="H190" s="2"/>
+    </row>
+    <row r="191" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E191" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="F186" s="2" t="s">
+      <c r="F191" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G186" s="2" t="s">
+      <c r="G191" s="2" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="187" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E187" s="2" t="s">
+      <c r="H191" s="2"/>
+    </row>
+    <row r="192" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E192" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="F187" s="2" t="s">
+      <c r="F192" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="G187" s="2" t="s">
+      <c r="G192" s="2" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="188" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E188" s="2" t="s">
+      <c r="H192" s="2"/>
+    </row>
+    <row r="193" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E193" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="F188" s="2" t="s">
+      <c r="F193" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="G188" s="2" t="s">
+      <c r="G193" s="2" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="189" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E189" s="2" t="s">
+      <c r="H193" s="2"/>
+    </row>
+    <row r="194" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E194" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="F189" s="2" t="s">
+      <c r="F194" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="G189" s="2" t="s">
+      <c r="G194" s="2" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="190" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E190" s="2" t="s">
+      <c r="H194" s="2"/>
+    </row>
+    <row r="195" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E195" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="F190" s="2" t="s">
+      <c r="F195" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="G190" s="2" t="s">
+      <c r="G195" s="2" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="191" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E191" s="2" t="s">
+      <c r="H195" s="2"/>
+    </row>
+    <row r="196" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E196" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="F191" s="2" t="s">
+      <c r="F196" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="G191" s="2" t="s">
+      <c r="G196" s="2" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="192" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E192" s="2" t="s">
+      <c r="H196" s="2"/>
+    </row>
+    <row r="197" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E197" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="F192" s="2" t="s">
+      <c r="F197" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="G192" s="2" t="s">
+      <c r="G197" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="193" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E193" s="2" t="s">
+      <c r="H197" s="2"/>
+    </row>
+    <row r="198" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E198" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="F193" s="2" t="s">
+      <c r="F198" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="G193" s="2" t="s">
+      <c r="G198" s="2" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="194" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E194" s="2" t="s">
+      <c r="H198" s="2"/>
+    </row>
+    <row r="199" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E199" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="F194" s="2" t="s">
+      <c r="F199" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="G194" s="2" t="s">
+      <c r="G199" s="2" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="195" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E195" s="2" t="s">
+      <c r="H199" s="2"/>
+    </row>
+    <row r="200" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E200" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="F195" s="2" t="s">
+      <c r="F200" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="G195" s="2" t="s">
+      <c r="G200" s="2" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="196" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E196" s="2" t="s">
+      <c r="H200" s="2"/>
+    </row>
+    <row r="201" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E201" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="F196" s="2" t="s">
+      <c r="F201" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="G196" s="2" t="s">
+      <c r="G201" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="197" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E197" s="2" t="s">
+      <c r="H201" s="2"/>
+    </row>
+    <row r="202" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E202" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="F197" s="2" t="s">
+      <c r="F202" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="G197" s="2" t="s">
+      <c r="G202" s="2" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="198" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E198" s="2" t="s">
+      <c r="H202" s="2"/>
+    </row>
+    <row r="203" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E203" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="F198" s="2" t="s">
+      <c r="F203" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="G198" s="2" t="s">
+      <c r="G203" s="2" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="199" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E199" s="2" t="s">
+      <c r="H203" s="2"/>
+    </row>
+    <row r="204" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E204" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="F199" s="2" t="s">
+      <c r="F204" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="G199" s="2" t="s">
+      <c r="G204" s="2" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="200" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E200" s="2" t="s">
+      <c r="H204" s="2"/>
+    </row>
+    <row r="205" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E205" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="F200" s="2" t="s">
+      <c r="F205" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="G200" s="2" t="s">
+      <c r="G205" s="2" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="201" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E201" s="2" t="s">
+      <c r="H205" s="2"/>
+    </row>
+    <row r="206" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E206" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="F201" s="2" t="s">
+      <c r="F206" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="G201" s="2" t="s">
+      <c r="G206" s="2" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="202" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E202" s="2" t="s">
+      <c r="H206" s="2"/>
+    </row>
+    <row r="207" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E207" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="F202" s="2" t="s">
+      <c r="F207" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="G202" s="2" t="s">
+      <c r="G207" s="2" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="203" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E203" s="2" t="s">
+      <c r="H207" s="2"/>
+    </row>
+    <row r="208" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E208" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="F203" s="2" t="s">
+      <c r="F208" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="G203" s="2" t="s">
+      <c r="G208" s="2" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="204" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E204" s="2" t="s">
+      <c r="H208" s="2"/>
+    </row>
+    <row r="209" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E209" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="F204" s="2" t="s">
+      <c r="F209" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G204" s="2" t="s">
+      <c r="G209" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="H209" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Added new book 18: WebScraping WikiPages using Python and listing into TreeView
</commit_message>
<xml_diff>
--- a/booksonline/FrameworkForJiraApi.xlsx
+++ b/booksonline/FrameworkForJiraApi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\Now\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F331C088-93BD-40BF-AB56-7358C129B19B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B767EBE3-BFBA-4B0D-A46F-DF8A6DC015DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2C462DE-B581-48D9-99D4-AC6A6E2A3CBA}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="__BW_TABLE_PROPERTIES">#REF!</definedName>
-    <definedName name="frameworkJiraApi">framework!$E$3:$H$209</definedName>
+    <definedName name="frameworkJiraApi">framework!$E$3:$G$204</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="605">
   <si>
     <t>Jira Resource</t>
   </si>
@@ -3649,54 +3649,6 @@
   </si>
   <si>
     <t>201. Issues</t>
-  </si>
-  <si>
-    <t>2.1 Isssues Assigned to current User across all projects</t>
-  </si>
-  <si>
-    <t>Returns issues from all project since your JQL does not include any project specific conditions.</t>
-  </si>
-  <si>
-    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee=currentuser()</t>
-  </si>
-  <si>
-    <t>Extract Information from JSON</t>
-  </si>
-  <si>
-    <t>2.2 Get all open issues by project</t>
-  </si>
-  <si>
-    <t>Get all open issues by project</t>
-  </si>
-  <si>
-    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee = 'akshay.dongave@boardwalktech.com' and project=10010 AND status in ("In Progress", "To Do") AND resolution = Unresolved order by updated DESC</t>
-  </si>
-  <si>
-    <t>2.3 Get all issue by issuetype in specific project</t>
-  </si>
-  <si>
-    <t>Get all issue by issuetype in specific project</t>
-  </si>
-  <si>
-    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee = 'akshay.dongave@boardwalktech.com' and project=10010 AND issuetype = Task AND status in ("In Progress", "To Do") AND resolution = Unresolved order by updated DESC</t>
-  </si>
-  <si>
-    <t>2.4 Get all unresolved issue by specific project</t>
-  </si>
-  <si>
-    <t>Get all unresolved issue by specific project</t>
-  </si>
-  <si>
-    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee in (currentUser()) AND project = UCW AND issuetype in standardIssueTypes() AND status in ("In Progress", "To Do") AND resolution = Unresolved ORDER BY created DESC</t>
-  </si>
-  <si>
-    <t>2.5 Get all resolved issue by specific project</t>
-  </si>
-  <si>
-    <t>Get all resolved issue by specific project</t>
-  </si>
-  <si>
-    <t>{JIRA_SERVER}/rest/api/2/search?jql=assignee in (currentUser()) AND project = UCW AND issuetype in standardIssueTypes() AND status in ("In Progress", "To Do") AND resolution = Done ORDER BY created DESC</t>
   </si>
 </sst>
 </file>
@@ -4091,10 +4043,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8241749-1F6A-48E6-B41D-93FEA9771075}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="E3:H209"/>
+  <dimension ref="E3:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4102,12 +4054,11 @@
     <col min="1" max="4" width="8.88671875" style="3"/>
     <col min="5" max="5" width="45.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="44.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="71.33203125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="71.33203125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4117,11 +4068,8 @@
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="4" spans="5:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E4" s="2" t="s">
         <v>404</v>
       </c>
@@ -4131,9 +4079,8 @@
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="5:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E5" s="2" t="s">
         <v>405</v>
       </c>
@@ -4143,2455 +4090,2195 @@
       <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="5:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E6" s="2" t="s">
-        <v>605</v>
+        <v>406</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>607</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="5:8" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E7" s="2" t="s">
-        <v>609</v>
+        <v>407</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>611</v>
+        <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="5:8" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E8" s="2" t="s">
-        <v>612</v>
+        <v>408</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>614</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="5:8" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E9" s="2" t="s">
-        <v>615</v>
+        <v>409</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>617</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="5:8" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E10" s="2" t="s">
-        <v>618</v>
+        <v>410</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>620</v>
+        <v>16</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="5:8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E11" s="2" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="5:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E12" s="2" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="5:8" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E13" s="2" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="5:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E14" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="5:8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E15" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="5:8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E16" s="2" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E17" s="2" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E18" s="2" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E19" s="2" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E20" s="2" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E21" s="2" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E22" s="2" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E23" s="2" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E24" s="2" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E25" s="2" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E26" s="2" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E27" s="2" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E28" s="2" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E29" s="2" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E30" s="2" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E31" s="2" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E32" s="2" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E33" s="2" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E34" s="2" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E35" s="2" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E36" s="2" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E37" s="2" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E38" s="2" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E39" s="2" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E40" s="2" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E41" s="2" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H41" s="2"/>
-    </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E42" s="2" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E43" s="2" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E44" s="2" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E45" s="2" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E46" s="2" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E47" s="2" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E48" s="2" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E49" s="2" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E50" s="2" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E51" s="2" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E52" s="2" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E53" s="2" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E54" s="2" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E55" s="2" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="5:8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E56" s="2" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="5:8" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E57" s="2" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="5:8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E58" s="2" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="5:8" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E59" s="2" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="5:8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E60" s="2" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="5:8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E61" s="2" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="5:8" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E62" s="2" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="5:8" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E63" s="2" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H63" s="2"/>
-    </row>
-    <row r="64" spans="5:8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E64" s="2" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E65" s="2" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E66" s="2" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E67" s="2" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E68" s="2" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E69" s="2" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E70" s="2" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="5:8" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E71" s="2" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="5:8" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E72" s="2" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H72" s="2"/>
-    </row>
-    <row r="73" spans="5:8" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E73" s="2" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H73" s="2"/>
-    </row>
-    <row r="74" spans="5:8" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E74" s="2" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H74" s="2"/>
-    </row>
-    <row r="75" spans="5:8" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E75" s="2" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H75" s="2"/>
-    </row>
-    <row r="76" spans="5:8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E76" s="2" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H76" s="2"/>
-    </row>
-    <row r="77" spans="5:8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E77" s="2" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H77" s="2"/>
-    </row>
-    <row r="78" spans="5:8" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E78" s="2" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H78" s="2"/>
-    </row>
-    <row r="79" spans="5:8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E79" s="2" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="H79" s="2"/>
-    </row>
-    <row r="80" spans="5:8" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E80" s="2" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H80" s="2"/>
-    </row>
-    <row r="81" spans="5:8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E81" s="2" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H81" s="2"/>
-    </row>
-    <row r="82" spans="5:8" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E82" s="2" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H82" s="2"/>
-    </row>
-    <row r="83" spans="5:8" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E83" s="2" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="H83" s="2"/>
-    </row>
-    <row r="84" spans="5:8" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E84" s="2" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="H84" s="2"/>
-    </row>
-    <row r="85" spans="5:8" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E85" s="2" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H85" s="2"/>
-    </row>
-    <row r="86" spans="5:8" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E86" s="2" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H86" s="2"/>
-    </row>
-    <row r="87" spans="5:8" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E87" s="2" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H87" s="2"/>
-    </row>
-    <row r="88" spans="5:8" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E88" s="2" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H88" s="2"/>
-    </row>
-    <row r="89" spans="5:8" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E89" s="2" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H89" s="2"/>
-    </row>
-    <row r="90" spans="5:8" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="90" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E90" s="2" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="H90" s="2"/>
-    </row>
-    <row r="91" spans="5:8" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="91" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E91" s="2" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H91" s="2"/>
-    </row>
-    <row r="92" spans="5:8" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="92" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E92" s="2" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H92" s="2"/>
-    </row>
-    <row r="93" spans="5:8" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E93" s="2" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H93" s="2"/>
-    </row>
-    <row r="94" spans="5:8" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="94" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E94" s="2" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="H94" s="2"/>
-    </row>
-    <row r="95" spans="5:8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="95" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E95" s="2" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="H95" s="2"/>
-    </row>
-    <row r="96" spans="5:8" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="96" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E96" s="2" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="5:8" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="97" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E97" s="2" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H97" s="2"/>
-    </row>
-    <row r="98" spans="5:8" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E98" s="2" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="5:8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E99" s="2" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H99" s="2"/>
-    </row>
-    <row r="100" spans="5:8" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="100" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E100" s="2" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H100" s="2"/>
-    </row>
-    <row r="101" spans="5:8" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="101" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E101" s="2" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H101" s="2"/>
-    </row>
-    <row r="102" spans="5:8" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="102" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E102" s="2" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H102" s="2"/>
-    </row>
-    <row r="103" spans="5:8" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E103" s="2" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H103" s="2"/>
-    </row>
-    <row r="104" spans="5:8" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E104" s="2" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H104" s="2"/>
-    </row>
-    <row r="105" spans="5:8" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="105" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E105" s="2" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H105" s="2"/>
-    </row>
-    <row r="106" spans="5:8" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E106" s="2" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H106" s="2"/>
-    </row>
-    <row r="107" spans="5:8" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E107" s="2" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="H107" s="2"/>
-    </row>
-    <row r="108" spans="5:8" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="108" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E108" s="2" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H108" s="2"/>
-    </row>
-    <row r="109" spans="5:8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="109" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E109" s="2" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H109" s="2"/>
-    </row>
-    <row r="110" spans="5:8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E110" s="2" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="H110" s="2"/>
-    </row>
-    <row r="111" spans="5:8" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="111" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E111" s="2" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H111" s="2"/>
-    </row>
-    <row r="112" spans="5:8" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="112" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E112" s="2" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H112" s="2"/>
-    </row>
-    <row r="113" spans="5:8" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="113" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E113" s="2" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H113" s="2"/>
-    </row>
-    <row r="114" spans="5:8" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="114" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E114" s="2" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="H114" s="2"/>
-    </row>
-    <row r="115" spans="5:8" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="115" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E115" s="2" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H115" s="2"/>
-    </row>
-    <row r="116" spans="5:8" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="116" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E116" s="2" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="H116" s="2"/>
-    </row>
-    <row r="117" spans="5:8" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="117" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E117" s="2" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="H117" s="2"/>
-    </row>
-    <row r="118" spans="5:8" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="118" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E118" s="2" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="H118" s="2"/>
-    </row>
-    <row r="119" spans="5:8" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="119" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E119" s="2" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="H119" s="2"/>
-    </row>
-    <row r="120" spans="5:8" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="120" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E120" s="2" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="H120" s="2"/>
-    </row>
-    <row r="121" spans="5:8" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="121" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E121" s="2" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="H121" s="2"/>
-    </row>
-    <row r="122" spans="5:8" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="122" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E122" s="2" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="H122" s="2"/>
-    </row>
-    <row r="123" spans="5:8" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="123" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E123" s="2" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="H123" s="2"/>
-    </row>
-    <row r="124" spans="5:8" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="124" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E124" s="2" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="H124" s="2"/>
-    </row>
-    <row r="125" spans="5:8" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="125" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E125" s="2" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H125" s="2"/>
-    </row>
-    <row r="126" spans="5:8" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="126" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E126" s="2" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="H126" s="2"/>
-    </row>
-    <row r="127" spans="5:8" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="127" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E127" s="2" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="H127" s="2"/>
-    </row>
-    <row r="128" spans="5:8" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="128" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E128" s="2" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="H128" s="2"/>
-    </row>
-    <row r="129" spans="5:8" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="129" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E129" s="2" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H129" s="2"/>
-    </row>
-    <row r="130" spans="5:8" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="130" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E130" s="2" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H130" s="2"/>
-    </row>
-    <row r="131" spans="5:8" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E131" s="2" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="H131" s="2"/>
-    </row>
-    <row r="132" spans="5:8" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="132" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E132" s="2" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="H132" s="2"/>
-    </row>
-    <row r="133" spans="5:8" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="133" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E133" s="2" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="H133" s="2"/>
-    </row>
-    <row r="134" spans="5:8" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="134" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E134" s="2" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="H134" s="2"/>
-    </row>
-    <row r="135" spans="5:8" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="135" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E135" s="2" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="H135" s="2"/>
-    </row>
-    <row r="136" spans="5:8" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="136" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E136" s="2" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="H136" s="2"/>
-    </row>
-    <row r="137" spans="5:8" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="137" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E137" s="2" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="H137" s="2"/>
-    </row>
-    <row r="138" spans="5:8" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="138" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E138" s="2" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="H138" s="2"/>
-    </row>
-    <row r="139" spans="5:8" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="139" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E139" s="2" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="H139" s="2"/>
-    </row>
-    <row r="140" spans="5:8" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="140" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E140" s="2" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="H140" s="2"/>
-    </row>
-    <row r="141" spans="5:8" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="141" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E141" s="2" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="H141" s="2"/>
-    </row>
-    <row r="142" spans="5:8" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="142" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E142" s="2" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="H142" s="2"/>
-    </row>
-    <row r="143" spans="5:8" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="143" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E143" s="2" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="H143" s="2"/>
-    </row>
-    <row r="144" spans="5:8" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="144" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E144" s="2" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="H144" s="2"/>
-    </row>
-    <row r="145" spans="5:8" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="145" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E145" s="2" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="H145" s="2"/>
-    </row>
-    <row r="146" spans="5:8" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="146" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E146" s="2" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="H146" s="2"/>
-    </row>
-    <row r="147" spans="5:8" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="147" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E147" s="2" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="H147" s="2"/>
-    </row>
-    <row r="148" spans="5:8" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="148" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E148" s="2" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="H148" s="2"/>
-    </row>
-    <row r="149" spans="5:8" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="149" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E149" s="2" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="H149" s="2"/>
-    </row>
-    <row r="150" spans="5:8" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="150" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E150" s="2" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="H150" s="2"/>
-    </row>
-    <row r="151" spans="5:8" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="151" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E151" s="2" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="H151" s="2"/>
-    </row>
-    <row r="152" spans="5:8" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="152" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E152" s="2" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="H152" s="2"/>
-    </row>
-    <row r="153" spans="5:8" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="153" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E153" s="2" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="H153" s="2"/>
-    </row>
-    <row r="154" spans="5:8" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="154" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E154" s="2" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="H154" s="2"/>
-    </row>
-    <row r="155" spans="5:8" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="155" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E155" s="2" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="H155" s="2"/>
-    </row>
-    <row r="156" spans="5:8" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="156" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E156" s="2" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="H156" s="2"/>
-    </row>
-    <row r="157" spans="5:8" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="157" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E157" s="2" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="H157" s="2"/>
-    </row>
-    <row r="158" spans="5:8" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="158" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E158" s="2" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="H158" s="2"/>
-    </row>
-    <row r="159" spans="5:8" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="159" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E159" s="2" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="H159" s="2"/>
-    </row>
-    <row r="160" spans="5:8" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="160" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E160" s="2" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="H160" s="2"/>
-    </row>
-    <row r="161" spans="5:8" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="161" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E161" s="2" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="H161" s="2"/>
-    </row>
-    <row r="162" spans="5:8" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="162" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E162" s="2" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="H162" s="2"/>
-    </row>
-    <row r="163" spans="5:8" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="163" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E163" s="2" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="H163" s="2"/>
-    </row>
-    <row r="164" spans="5:8" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="164" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E164" s="2" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="H164" s="2"/>
-    </row>
-    <row r="165" spans="5:8" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="165" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E165" s="2" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="H165" s="2"/>
-    </row>
-    <row r="166" spans="5:8" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="166" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E166" s="2" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="H166" s="2"/>
-    </row>
-    <row r="167" spans="5:8" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="167" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E167" s="2" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="H167" s="2"/>
-    </row>
-    <row r="168" spans="5:8" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="168" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E168" s="2" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="H168" s="2"/>
-    </row>
-    <row r="169" spans="5:8" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="169" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E169" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H169" s="2"/>
-    </row>
-    <row r="170" spans="5:8" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="170" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E170" s="2" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="H170" s="2"/>
-    </row>
-    <row r="171" spans="5:8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="171" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E171" s="2" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="H171" s="2"/>
-    </row>
-    <row r="172" spans="5:8" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="172" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E172" s="2" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="H172" s="2"/>
-    </row>
-    <row r="173" spans="5:8" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="173" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E173" s="2" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="H173" s="2"/>
-    </row>
-    <row r="174" spans="5:8" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="174" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E174" s="2" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="H174" s="2"/>
-    </row>
-    <row r="175" spans="5:8" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="175" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E175" s="2" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="H175" s="2"/>
-    </row>
-    <row r="176" spans="5:8" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="176" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E176" s="2" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="H176" s="2"/>
-    </row>
-    <row r="177" spans="5:8" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="177" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E177" s="2" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="H177" s="2"/>
-    </row>
-    <row r="178" spans="5:8" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="178" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E178" s="2" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="H178" s="2"/>
-    </row>
-    <row r="179" spans="5:8" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="179" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E179" s="2" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="H179" s="2"/>
-    </row>
-    <row r="180" spans="5:8" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="180" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E180" s="2" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="H180" s="2"/>
-    </row>
-    <row r="181" spans="5:8" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="181" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E181" s="2" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="H181" s="2"/>
-    </row>
-    <row r="182" spans="5:8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="182" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E182" s="2" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="H182" s="2"/>
-    </row>
-    <row r="183" spans="5:8" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="183" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E183" s="2" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="H183" s="2"/>
-    </row>
-    <row r="184" spans="5:8" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="184" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E184" s="2" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="H184" s="2"/>
-    </row>
-    <row r="185" spans="5:8" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="185" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E185" s="2" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="F185" s="2" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="H185" s="2"/>
-    </row>
-    <row r="186" spans="5:8" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="186" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E186" s="2" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="F186" s="2" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="H186" s="2"/>
-    </row>
-    <row r="187" spans="5:8" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="187" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E187" s="2" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="F187" s="2" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H187" s="2"/>
-    </row>
-    <row r="188" spans="5:8" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="188" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E188" s="2" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="F188" s="2" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="H188" s="2"/>
-    </row>
-    <row r="189" spans="5:8" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="189" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E189" s="2" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="F189" s="2" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H189" s="2"/>
-    </row>
-    <row r="190" spans="5:8" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="190" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E190" s="2" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="H190" s="2"/>
-    </row>
-    <row r="191" spans="5:8" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="191" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E191" s="2" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H191" s="2"/>
-    </row>
-    <row r="192" spans="5:8" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="192" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E192" s="2" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="H192" s="2"/>
-    </row>
-    <row r="193" spans="5:8" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="193" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E193" s="2" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="F193" s="2" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="H193" s="2"/>
-    </row>
-    <row r="194" spans="5:8" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="194" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E194" s="2" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="F194" s="2" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="H194" s="2"/>
-    </row>
-    <row r="195" spans="5:8" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="195" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E195" s="2" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="F195" s="2" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="H195" s="2"/>
-    </row>
-    <row r="196" spans="5:8" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="196" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E196" s="2" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="H196" s="2"/>
-    </row>
-    <row r="197" spans="5:8" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="197" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E197" s="2" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="F197" s="2" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H197" s="2"/>
-    </row>
-    <row r="198" spans="5:8" x14ac:dyDescent="0.3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="198" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E198" s="2" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="H198" s="2"/>
-    </row>
-    <row r="199" spans="5:8" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="199" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E199" s="2" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="F199" s="2" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="H199" s="2"/>
-    </row>
-    <row r="200" spans="5:8" x14ac:dyDescent="0.3">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="200" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E200" s="2" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="F200" s="2" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="H200" s="2"/>
-    </row>
-    <row r="201" spans="5:8" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="201" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E201" s="2" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="F201" s="2" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="H201" s="2"/>
-    </row>
-    <row r="202" spans="5:8" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="202" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E202" s="2" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="F202" s="2" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="H202" s="2"/>
-    </row>
-    <row r="203" spans="5:8" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="203" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E203" s="2" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="F203" s="2" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="G203" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="H203" s="2"/>
-    </row>
-    <row r="204" spans="5:8" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="204" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E204" s="2" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="F204" s="2" t="s">
-        <v>395</v>
+        <v>6</v>
       </c>
       <c r="G204" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="H204" s="2"/>
-    </row>
-    <row r="205" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E205" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="F205" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="G205" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="H205" s="2"/>
-    </row>
-    <row r="206" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E206" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="F206" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="G206" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="H206" s="2"/>
-    </row>
-    <row r="207" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E207" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="F207" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="G207" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="H207" s="2"/>
-    </row>
-    <row r="208" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E208" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="F208" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="G208" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="H208" s="2"/>
-    </row>
-    <row r="209" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E209" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="F209" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G209" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H209" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>